<commit_message>
Cleaned up EC2 benchmarks and added scaleout.
</commit_message>
<xml_diff>
--- a/benchmark-ec2.xlsx
+++ b/benchmark-ec2.xlsx
@@ -4,28 +4,50 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="14565" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="run" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset" sheetId="2" r:id="rId1"/>
+    <sheet name="scaleout" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
-    <t>Num Points</t>
+    <t>Speedup</t>
   </si>
   <si>
-    <t>Time</t>
+    <t>Manipulation</t>
   </si>
   <si>
-    <t>StdDev</t>
+    <t>Points</t>
   </si>
   <si>
-    <t>2 Large High-Memory machines, varying dataset size</t>
+    <t>Times for each trial</t>
+  </si>
+  <si>
+    <t>Average time</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Slaves</t>
+  </si>
+  <si>
+    <t>Dataset size (MB)</t>
+  </si>
+  <si>
+    <t>2 Large slave instances, varying dataset size</t>
+  </si>
+  <si>
+    <t>Varying number of Large slave instances, 10,000,000 points</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
   </si>
 </sst>
 </file>
@@ -510,9 +532,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -583,6 +609,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iteration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> times for varying dataset size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -597,15 +643,24 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>run!$I$2</c:f>
+              <c:f>dataset!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time</c:v>
+                  <c:v>Average time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -613,201 +668,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>run!$J$3:$J$7</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.72340133842318866</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.25577243414262357</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.82686571294818956</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.2303687962709156</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.7021318196800492</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>run!$J$3:$J$7</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>0.72340133842318866</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.25577243414262357</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.82686571294818956</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.2303687962709156</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.7021318196800492</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
-            <c:noEndCap val="0"/>
-            <c:val val="1"/>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>run!$B$3:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>160000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>run!$I$3:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.741750701</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.3532705503333329</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.222430429000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28.050695524999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>59.186266179500002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="93243264"/>
-        <c:axId val="92858240"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="93243264"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92858240"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="92858240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93243264"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>run!$J$11:$J$19</c:f>
+                <c:f>dataset!$K$3:$K$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
@@ -843,7 +704,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>run!$J$11:$J$19</c:f>
+                <c:f>dataset!$K$3:$K$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
@@ -887,7 +748,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>run!$B$11:$B$19</c:f>
+              <c:f>dataset!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -923,9 +784,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>run!$I$11:$I$19</c:f>
+              <c:f>dataset!$J$3:$J$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4.9827379105</c:v>
@@ -967,11 +828,190 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81504512"/>
-        <c:axId val="61459072"/>
+        <c:axId val="100600064"/>
+        <c:axId val="106213760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81504512"/>
+        <c:axId val="100600064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Dataset size (2D</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> points, 128 bits each)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="106213760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="106213760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Time per iteration</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100600064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scaleout!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scaleout!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scaleout!$Q$3:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2017127246030244</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3630967857163387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="117139328"/>
+        <c:axId val="117137792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="117139328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,12 +1021,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61459072"/>
+        <c:crossAx val="117137792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61459072"/>
+        <c:axId val="117137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1037,316 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81504512"/>
+        <c:crossAx val="117139328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scaleout!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>scaleout!$P$3:$P$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>72.727390265212065</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>22.999814908543954</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18.734600192459254</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>scaleout!$P$3:$P$5</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>72.727390265212065</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>22.999814908543954</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18.734600192459254</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scaleout!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scaleout!$O$3:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>99.852217517583355</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.352064509499996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.690557209555557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="44963328"/>
+        <c:axId val="44961792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="44963328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44961792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="44961792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44963328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scaleout!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scaleout!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scaleout!$R$3:$R$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1008563623015122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84077419642908469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="49803648"/>
+        <c:axId val="48999040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="49803648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48999040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="48999040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49803648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1023,20 +1372,57 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1053,20 +1439,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1076,6 +1462,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1371,34 +1787,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1406,486 +1850,591 @@
         <f>POWER(2,A3)*10000000</f>
         <v>10000000</v>
       </c>
-      <c r="C3">
-        <v>5.4435562830000004</v>
-      </c>
-      <c r="D3">
-        <v>4.0263546410000002</v>
-      </c>
-      <c r="E3">
-        <v>5.3132387889999997</v>
-      </c>
-      <c r="F3">
-        <v>3.9112412839999999</v>
-      </c>
-      <c r="G3">
-        <v>5.6135942500000002</v>
-      </c>
-      <c r="H3">
-        <v>4.1425189590000002</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE(C3:H3)</f>
-        <v>4.741750701</v>
-      </c>
-      <c r="J3">
-        <f>_xlfn.STDEV.P(C3:H3)</f>
-        <v>0.72340133842318866</v>
+      <c r="C3" s="1">
+        <f>B3*16/(1024*1024)</f>
+        <v>152.587890625</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5.4375119959999996</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3.8840241550000001</v>
+      </c>
+      <c r="F3" s="3">
+        <v>5.5053185449999997</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5.4332874249999996</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5.4905620119999998</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4.14572333</v>
+      </c>
+      <c r="J3" s="3">
+        <f>AVERAGE(D3:I3)</f>
+        <v>4.9827379105</v>
+      </c>
+      <c r="K3" s="3">
+        <f>_xlfn.STDEV.P(D3:I3)</f>
+        <v>0.68902775657343995</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B7" si="0">POWER(2,A4)*10000000</f>
+        <f>POWER(2,A4)*10000000</f>
         <v>20000000</v>
       </c>
-      <c r="C4">
-        <v>8.6538593059999993</v>
-      </c>
-      <c r="D4">
-        <v>8.3612181069999991</v>
-      </c>
-      <c r="E4">
-        <v>8.5109771260000002</v>
-      </c>
-      <c r="F4">
-        <v>7.9931962570000001</v>
-      </c>
-      <c r="G4">
-        <v>8.5665879409999999</v>
-      </c>
-      <c r="H4">
-        <v>8.0337845649999995</v>
-      </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I7" si="1">AVERAGE(C4:H4)</f>
-        <v>8.3532705503333329</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J7" si="2">_xlfn.STDEV.P(C4:H4)</f>
-        <v>0.25577243414262357</v>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C11" si="0">B4*16/(1024*1024)</f>
+        <v>305.17578125</v>
+      </c>
+      <c r="D4" s="3">
+        <v>30.369976542</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8.1473263110000005</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8.6581077969999996</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7.8919247989999999</v>
+      </c>
+      <c r="H4" s="3">
+        <v>13.073602111</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7.9497464170000001</v>
+      </c>
+      <c r="J4" s="3">
+        <f>AVERAGE(D4:I4)</f>
+        <v>12.681780662833333</v>
+      </c>
+      <c r="K4" s="3">
+        <f>_xlfn.STDEV.P(D4:I4)</f>
+        <v>8.1149233350984673</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" s="1">
+        <f>POWER(2,A5)*10000000</f>
+        <v>40000000</v>
+      </c>
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>40000000</v>
-      </c>
-      <c r="C5">
-        <v>16.693034592</v>
-      </c>
-      <c r="D5">
-        <v>17.058480659000001</v>
-      </c>
-      <c r="E5">
-        <v>15.168912905999999</v>
-      </c>
-      <c r="F5">
-        <v>14.989145182</v>
-      </c>
-      <c r="G5">
-        <v>16.524680116999999</v>
-      </c>
-      <c r="H5">
-        <v>16.900329117999998</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>16.222430429000003</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0.82686571294818956</v>
+        <v>610.3515625</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16.681410463999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>16.234956396000001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>14.576628547</v>
+      </c>
+      <c r="G5" s="3">
+        <v>14.785649045</v>
+      </c>
+      <c r="H5" s="3">
+        <v>14.852692257999999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>14.376864793999999</v>
+      </c>
+      <c r="J5" s="3">
+        <f>AVERAGE(D5:I5)</f>
+        <v>15.251366917333334</v>
+      </c>
+      <c r="K5" s="3">
+        <f>_xlfn.STDEV.P(D5:I5)</f>
+        <v>0.87638778142883877</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="1">
+        <f>POWER(2,A6)*10000000</f>
+        <v>80000000</v>
+      </c>
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>80000000</v>
-      </c>
-      <c r="C6">
-        <v>27.445370504</v>
-      </c>
-      <c r="D6">
-        <v>26.479855752999999</v>
-      </c>
-      <c r="E6">
-        <v>27.061461036000001</v>
-      </c>
-      <c r="F6">
-        <v>28.418928529999999</v>
-      </c>
-      <c r="G6">
-        <v>28.667409663000001</v>
-      </c>
-      <c r="H6">
-        <v>30.231147664000002</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>28.050695524999998</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>1.2303687962709156</v>
+        <v>1220.703125</v>
+      </c>
+      <c r="D6" s="3">
+        <v>30.308659379000002</v>
+      </c>
+      <c r="E6" s="3">
+        <v>28.062001976000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>27.704078054</v>
+      </c>
+      <c r="G6" s="3">
+        <v>27.920177889000001</v>
+      </c>
+      <c r="H6" s="3">
+        <v>29.578870388999999</v>
+      </c>
+      <c r="I6" s="3">
+        <v>28.187332365</v>
+      </c>
+      <c r="J6" s="3">
+        <f>AVERAGE(D6:I6)</f>
+        <v>28.626853342</v>
+      </c>
+      <c r="K6" s="3">
+        <f>_xlfn.STDEV.P(D6:I6)</f>
+        <v>0.96591478115994478</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" s="1">
+        <f>POWER(2,A7)*10000000</f>
+        <v>160000000</v>
+      </c>
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>160000000</v>
-      </c>
-      <c r="C7">
-        <v>60.039829881000003</v>
-      </c>
-      <c r="D7">
-        <v>62.203804728999998</v>
-      </c>
-      <c r="E7">
-        <v>57.786429159999997</v>
-      </c>
-      <c r="F7">
-        <v>62.815610159000002</v>
-      </c>
-      <c r="G7">
-        <v>55.793477588999998</v>
-      </c>
-      <c r="H7">
-        <v>56.478445559000001</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>59.186266179500002</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>2.7021318196800492</v>
+        <v>2441.40625</v>
+      </c>
+      <c r="D7" s="3">
+        <v>56.206809589000002</v>
+      </c>
+      <c r="E7" s="3">
+        <v>57.000327378999998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>59.753585678999997</v>
+      </c>
+      <c r="G7" s="3">
+        <v>58.725397876000002</v>
+      </c>
+      <c r="H7" s="3">
+        <v>58.818541207000003</v>
+      </c>
+      <c r="I7" s="3">
+        <v>59.288726250000003</v>
+      </c>
+      <c r="J7" s="3">
+        <f>AVERAGE(D7:I7)</f>
+        <v>58.298897996666675</v>
+      </c>
+      <c r="K7" s="3">
+        <f>_xlfn.STDEV.P(D7:I7)</f>
+        <v>1.265630738137218</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <f>POWER(2,A8)*10000000</f>
+        <v>320000000</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>4882.8125</v>
+      </c>
+      <c r="D8" s="3">
+        <v>121.00197950800001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>135.91639437699999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>114.772993345</v>
+      </c>
+      <c r="G8" s="3">
+        <v>130.70799132400001</v>
+      </c>
+      <c r="H8" s="3">
+        <v>117.68821961800001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>140.898986036</v>
+      </c>
+      <c r="J8" s="3">
+        <f>AVERAGE(D8:I8)</f>
+        <v>126.83109403466665</v>
+      </c>
+      <c r="K8" s="3">
+        <f>_xlfn.STDEV.P(D8:I8)</f>
+        <v>9.647513680302076</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <f>POWER(2,A9)*10000000</f>
+        <v>640000000</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>9765.625</v>
+      </c>
+      <c r="D9" s="3">
+        <v>236.702653707</v>
+      </c>
+      <c r="E9" s="3">
+        <v>246.078785716</v>
+      </c>
+      <c r="F9" s="3">
+        <v>237.002679242</v>
+      </c>
+      <c r="G9" s="3">
+        <v>242.5779775</v>
+      </c>
+      <c r="H9" s="3">
+        <v>264.16699282799999</v>
+      </c>
+      <c r="I9" s="3">
+        <v>248.460513695</v>
+      </c>
+      <c r="J9" s="3">
+        <f>AVERAGE(D9:I9)</f>
+        <v>245.83160044799999</v>
+      </c>
+      <c r="K9" s="3">
+        <f>_xlfn.STDEV.P(D9:I9)</f>
+        <v>9.2649202163775932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <f>POWER(2,A10)*10000000</f>
+        <v>1280000000</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>19531.25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>525.49750017999997</v>
+      </c>
+      <c r="E10" s="3">
+        <v>506.82523131300002</v>
+      </c>
+      <c r="F10" s="3">
+        <v>511.57142558300001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>520.49130418799996</v>
+      </c>
+      <c r="H10" s="3">
+        <v>495.57018852800002</v>
+      </c>
+      <c r="I10" s="3">
+        <v>527.18513592900001</v>
+      </c>
+      <c r="J10" s="3">
+        <f>AVERAGE(D10:I10)</f>
+        <v>514.52346428683325</v>
+      </c>
+      <c r="K10" s="3">
+        <f>_xlfn.STDEV.P(D10:I10)</f>
+        <v>11.132284065300325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <f>POWER(2,A11)*10000000</f>
-        <v>10000000</v>
-      </c>
-      <c r="C11">
-        <v>5.4375119959999996</v>
-      </c>
-      <c r="D11">
-        <v>3.8840241550000001</v>
-      </c>
-      <c r="E11">
-        <v>5.5053185449999997</v>
-      </c>
-      <c r="F11">
-        <v>5.4332874249999996</v>
-      </c>
-      <c r="G11">
-        <v>5.4905620119999998</v>
-      </c>
-      <c r="H11">
-        <v>4.14572333</v>
-      </c>
-      <c r="I11">
-        <f>AVERAGE(C11:H11)</f>
-        <v>4.9827379105</v>
-      </c>
-      <c r="J11">
-        <f>_xlfn.STDEV.P(C11:H11)</f>
-        <v>0.68902775657343995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" ref="B12:B19" si="3">POWER(2,A12)*10000000</f>
-        <v>20000000</v>
-      </c>
-      <c r="C12">
-        <v>30.369976542</v>
-      </c>
-      <c r="D12">
-        <v>8.1473263110000005</v>
-      </c>
-      <c r="E12">
-        <v>8.6581077969999996</v>
-      </c>
-      <c r="F12">
-        <v>7.8919247989999999</v>
-      </c>
-      <c r="G12">
-        <v>13.073602111</v>
-      </c>
-      <c r="H12">
-        <v>7.9497464170000001</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ref="I12:I19" si="4">AVERAGE(C12:H12)</f>
-        <v>12.681780662833333</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ref="J12:J19" si="5">_xlfn.STDEV.P(C12:H12)</f>
-        <v>8.1149233350984673</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <f t="shared" si="3"/>
-        <v>40000000</v>
-      </c>
-      <c r="C13">
-        <v>16.681410463999999</v>
-      </c>
-      <c r="D13">
-        <v>16.234956396000001</v>
-      </c>
-      <c r="E13">
-        <v>14.576628547</v>
-      </c>
-      <c r="F13">
-        <v>14.785649045</v>
-      </c>
-      <c r="G13">
-        <v>14.852692257999999</v>
-      </c>
-      <c r="H13">
-        <v>14.376864793999999</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="4"/>
-        <v>15.251366917333334</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>0.87638778142883877</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1">
-        <f t="shared" si="3"/>
-        <v>80000000</v>
-      </c>
-      <c r="C14">
-        <v>30.308659379000002</v>
-      </c>
-      <c r="D14">
-        <v>28.062001976000001</v>
-      </c>
-      <c r="E14">
-        <v>27.704078054</v>
-      </c>
-      <c r="F14">
-        <v>27.920177889000001</v>
-      </c>
-      <c r="G14">
-        <v>29.578870388999999</v>
-      </c>
-      <c r="H14">
-        <v>28.187332365</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="4"/>
-        <v>28.626853342</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>0.96591478115994478</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <f t="shared" si="3"/>
-        <v>160000000</v>
-      </c>
-      <c r="C15">
-        <v>56.206809589000002</v>
-      </c>
-      <c r="D15">
-        <v>57.000327378999998</v>
-      </c>
-      <c r="E15">
-        <v>59.753585678999997</v>
-      </c>
-      <c r="F15">
-        <v>58.725397876000002</v>
-      </c>
-      <c r="G15">
-        <v>58.818541207000003</v>
-      </c>
-      <c r="H15">
-        <v>59.288726250000003</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="4"/>
-        <v>58.298897996666675</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>1.265630738137218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" si="3"/>
-        <v>320000000</v>
-      </c>
-      <c r="C16">
-        <v>121.00197950800001</v>
-      </c>
-      <c r="D16">
-        <v>135.91639437699999</v>
-      </c>
-      <c r="E16">
-        <v>114.772993345</v>
-      </c>
-      <c r="F16">
-        <v>130.70799132400001</v>
-      </c>
-      <c r="G16">
-        <v>117.68821961800001</v>
-      </c>
-      <c r="H16">
-        <v>140.898986036</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="4"/>
-        <v>126.83109403466665</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>9.647513680302076</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1">
-        <f t="shared" si="3"/>
-        <v>640000000</v>
-      </c>
-      <c r="C17">
-        <v>236.702653707</v>
-      </c>
-      <c r="D17">
-        <v>246.078785716</v>
-      </c>
-      <c r="E17">
-        <v>237.002679242</v>
-      </c>
-      <c r="F17">
-        <v>242.5779775</v>
-      </c>
-      <c r="G17">
-        <v>264.16699282799999</v>
-      </c>
-      <c r="H17">
-        <v>248.460513695</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="4"/>
-        <v>245.83160044799999</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="5"/>
-        <v>9.2649202163775932</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1">
-        <f t="shared" si="3"/>
-        <v>1280000000</v>
-      </c>
-      <c r="C18">
-        <v>525.49750017999997</v>
-      </c>
-      <c r="D18">
-        <v>506.82523131300002</v>
-      </c>
-      <c r="E18">
-        <v>511.57142558300001</v>
-      </c>
-      <c r="F18">
-        <v>520.49130418799996</v>
-      </c>
-      <c r="G18">
-        <v>495.57018852800002</v>
-      </c>
-      <c r="H18">
-        <v>527.18513592900001</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="4"/>
-        <v>514.52346428683325</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="5"/>
-        <v>11.132284065300325</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1">
-        <f t="shared" si="3"/>
         <v>2560000000</v>
       </c>
-      <c r="C19">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>39062.5</v>
+      </c>
+      <c r="D11" s="3">
         <v>997.88241648200005</v>
       </c>
-      <c r="D19">
+      <c r="E11" s="3">
         <v>1014.7266419809999</v>
       </c>
-      <c r="E19">
+      <c r="F11" s="3">
         <v>1005.472644829</v>
       </c>
-      <c r="F19">
+      <c r="G11" s="3">
         <v>1062.941862573</v>
       </c>
-      <c r="G19">
+      <c r="H11" s="3">
         <v>1051.812781742</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3">
+        <f>AVERAGE(D11:I11)</f>
         <v>1026.5672695214002</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
+      <c r="K11" s="3">
+        <f>_xlfn.STDEV.P(D11:I11)</f>
         <v>25.955544117993867</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B5" si="0">POWER(2,A3)</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>35.211869771000003</v>
+      </c>
+      <c r="D3">
+        <v>35.323963046999999</v>
+      </c>
+      <c r="E3">
+        <v>84.802126837000003</v>
+      </c>
+      <c r="F3">
+        <v>238.67107822200001</v>
+      </c>
+      <c r="G3">
+        <v>34.948073843000003</v>
+      </c>
+      <c r="H3">
+        <v>124.926804766</v>
+      </c>
+      <c r="I3">
+        <v>210.66634612799999</v>
+      </c>
+      <c r="J3">
+        <v>197.21022547800001</v>
+      </c>
+      <c r="K3">
+        <v>37.582094703999999</v>
+      </c>
+      <c r="L3">
+        <v>63.349654055000002</v>
+      </c>
+      <c r="M3">
+        <v>38.074690228000001</v>
+      </c>
+      <c r="N3">
+        <v>97.459683131999995</v>
+      </c>
+      <c r="O3">
+        <f>AVERAGE(C3:N3)</f>
+        <v>99.852217517583355</v>
+      </c>
+      <c r="P3">
+        <f>_xlfn.STDEV.P(C3:N3)</f>
+        <v>72.727390265212065</v>
+      </c>
+      <c r="Q3">
+        <f>O$3/O3</f>
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <f>Q3/(B3/B$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>24.670772554999999</v>
+      </c>
+      <c r="D4">
+        <v>25.749868376999999</v>
+      </c>
+      <c r="E4">
+        <v>91.027537190000004</v>
+      </c>
+      <c r="F4">
+        <v>42.400613149999998</v>
+      </c>
+      <c r="G4">
+        <v>32.641606121000002</v>
+      </c>
+      <c r="H4">
+        <v>55.621989663999997</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O5" si="1">AVERAGE(C4:N4)</f>
+        <v>45.352064509499996</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P5" si="2">_xlfn.STDEV.P(C4:N4)</f>
+        <v>22.999814908543954</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q5" si="3">O$3/O4</f>
+        <v>2.2017127246030244</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R5" si="4">Q4/(B4/B$3)</f>
+        <v>1.1008563623015122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>76.016092462000003</v>
+      </c>
+      <c r="D5">
+        <v>11.209864572000001</v>
+      </c>
+      <c r="E5">
+        <v>11.812956002</v>
+      </c>
+      <c r="F5">
+        <v>36.855980676999998</v>
+      </c>
+      <c r="G5">
+        <v>27.064551217000002</v>
+      </c>
+      <c r="H5">
+        <v>27.970506633999999</v>
+      </c>
+      <c r="I5">
+        <v>33.545485868</v>
+      </c>
+      <c r="J5">
+        <v>29.650450882000001</v>
+      </c>
+      <c r="K5">
+        <v>13.089126572</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>29.690557209555557</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>18.734600192459254</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>3.3630967857163387</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="4"/>
+        <v>0.84077419642908469</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="C2:N2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Finished report and benchmarks for last Spark meeting
</commit_message>
<xml_diff>
--- a/benchmark-ec2.xlsx
+++ b/benchmark-ec2.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="14565" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="14565"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="2" r:id="rId1"/>
     <sheet name="scaleout" sheetId="1" r:id="rId2"/>
+    <sheet name="scaleup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Speedup</t>
   </si>
@@ -44,10 +45,13 @@
     <t>2 Large slave instances, varying dataset size</t>
   </si>
   <si>
-    <t>Varying number of Large slave instances, 10,000,000 points</t>
+    <t>Efficiency</t>
   </si>
   <si>
-    <t>Efficiency</t>
+    <t>Varying number of Large slave instances, 100,000,000 points</t>
+  </si>
+  <si>
+    <t>Number of S</t>
   </si>
 </sst>
 </file>
@@ -535,10 +539,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -828,11 +832,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100600064"/>
-        <c:axId val="106213760"/>
+        <c:axId val="97403264"/>
+        <c:axId val="97405184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100600064"/>
+        <c:axId val="97403264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,12 +870,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106213760"/>
+        <c:crossAx val="97405184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106213760"/>
+        <c:axId val="97405184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +910,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100600064"/>
+        <c:crossAx val="97403264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1007,11 +1011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="117139328"/>
-        <c:axId val="117137792"/>
+        <c:axId val="97618560"/>
+        <c:axId val="97620352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="117139328"/>
+        <c:axId val="97618560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,12 +1025,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117137792"/>
+        <c:crossAx val="97620352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117137792"/>
+        <c:axId val="97620352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,7 +1041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117139328"/>
+        <c:crossAx val="97618560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1185,11 +1189,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44963328"/>
-        <c:axId val="44961792"/>
+        <c:axId val="97641216"/>
+        <c:axId val="97642752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44963328"/>
+        <c:axId val="97641216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,12 +1203,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44961792"/>
+        <c:crossAx val="97642752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44961792"/>
+        <c:axId val="97642752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,7 +1219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44963328"/>
+        <c:crossAx val="97641216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1316,11 +1320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49803648"/>
-        <c:axId val="48999040"/>
+        <c:axId val="97687424"/>
+        <c:axId val="97688960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49803648"/>
+        <c:axId val="97687424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,12 +1334,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48999040"/>
+        <c:crossAx val="97688960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48999040"/>
+        <c:axId val="97688960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1346,7 +1350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49803648"/>
+        <c:crossAx val="97687424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1789,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,19 +1807,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1827,14 +1831,14 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2" t="s">
         <v>4</v>
       </c>
@@ -1847,37 +1851,37 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <f>POWER(2,A3)*10000000</f>
+        <f t="shared" ref="B3:B11" si="0">POWER(2,A3)*10000000</f>
         <v>10000000</v>
       </c>
       <c r="C3" s="1">
         <f>B3*16/(1024*1024)</f>
         <v>152.587890625</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>5.4375119959999996</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>3.8840241550000001</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>5.5053185449999997</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>5.4332874249999996</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>5.4905620119999998</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>4.14572333</v>
       </c>
-      <c r="J3" s="3">
-        <f>AVERAGE(D3:I3)</f>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J11" si="1">AVERAGE(D3:I3)</f>
         <v>4.9827379105</v>
       </c>
-      <c r="K3" s="3">
-        <f>_xlfn.STDEV.P(D3:I3)</f>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K11" si="2">_xlfn.STDEV.P(D3:I3)</f>
         <v>0.68902775657343995</v>
       </c>
     </row>
@@ -1886,37 +1890,37 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <f>POWER(2,A4)*10000000</f>
+        <f t="shared" si="0"/>
         <v>20000000</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C11" si="0">B4*16/(1024*1024)</f>
+        <f t="shared" ref="C4:C11" si="3">B4*16/(1024*1024)</f>
         <v>305.17578125</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>30.369976542</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>8.1473263110000005</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>8.6581077969999996</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>7.8919247989999999</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>13.073602111</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>7.9497464170000001</v>
       </c>
-      <c r="J4" s="3">
-        <f>AVERAGE(D4:I4)</f>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
         <v>12.681780662833333</v>
       </c>
-      <c r="K4" s="3">
-        <f>_xlfn.STDEV.P(D4:I4)</f>
+      <c r="K4" s="2">
+        <f t="shared" si="2"/>
         <v>8.1149233350984673</v>
       </c>
     </row>
@@ -1925,37 +1929,37 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <f>POWER(2,A5)*10000000</f>
+        <f t="shared" si="0"/>
         <v>40000000</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>610.3515625</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>16.681410463999999</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>16.234956396000001</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>14.576628547</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>14.785649045</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>14.852692257999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>14.376864793999999</v>
       </c>
-      <c r="J5" s="3">
-        <f>AVERAGE(D5:I5)</f>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
         <v>15.251366917333334</v>
       </c>
-      <c r="K5" s="3">
-        <f>_xlfn.STDEV.P(D5:I5)</f>
+      <c r="K5" s="2">
+        <f t="shared" si="2"/>
         <v>0.87638778142883877</v>
       </c>
     </row>
@@ -1964,37 +1968,37 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <f>POWER(2,A6)*10000000</f>
+        <f t="shared" si="0"/>
         <v>80000000</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1220.703125</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>30.308659379000002</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>28.062001976000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>27.704078054</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>27.920177889000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>29.578870388999999</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>28.187332365</v>
       </c>
-      <c r="J6" s="3">
-        <f>AVERAGE(D6:I6)</f>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
         <v>28.626853342</v>
       </c>
-      <c r="K6" s="3">
-        <f>_xlfn.STDEV.P(D6:I6)</f>
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
         <v>0.96591478115994478</v>
       </c>
     </row>
@@ -2003,37 +2007,37 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <f>POWER(2,A7)*10000000</f>
+        <f t="shared" si="0"/>
         <v>160000000</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2441.40625</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>56.206809589000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>57.000327378999998</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>59.753585678999997</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>58.725397876000002</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>58.818541207000003</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>59.288726250000003</v>
       </c>
-      <c r="J7" s="3">
-        <f>AVERAGE(D7:I7)</f>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
         <v>58.298897996666675</v>
       </c>
-      <c r="K7" s="3">
-        <f>_xlfn.STDEV.P(D7:I7)</f>
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
         <v>1.265630738137218</v>
       </c>
     </row>
@@ -2042,37 +2046,37 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <f>POWER(2,A8)*10000000</f>
+        <f t="shared" si="0"/>
         <v>320000000</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4882.8125</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>121.00197950800001</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>135.91639437699999</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>114.772993345</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>130.70799132400001</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>117.68821961800001</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>140.898986036</v>
       </c>
-      <c r="J8" s="3">
-        <f>AVERAGE(D8:I8)</f>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
         <v>126.83109403466665</v>
       </c>
-      <c r="K8" s="3">
-        <f>_xlfn.STDEV.P(D8:I8)</f>
+      <c r="K8" s="2">
+        <f t="shared" si="2"/>
         <v>9.647513680302076</v>
       </c>
     </row>
@@ -2081,37 +2085,37 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <f>POWER(2,A9)*10000000</f>
+        <f t="shared" si="0"/>
         <v>640000000</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9765.625</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>236.702653707</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>246.078785716</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>237.002679242</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>242.5779775</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>264.16699282799999</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>248.460513695</v>
       </c>
-      <c r="J9" s="3">
-        <f>AVERAGE(D9:I9)</f>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
         <v>245.83160044799999</v>
       </c>
-      <c r="K9" s="3">
-        <f>_xlfn.STDEV.P(D9:I9)</f>
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
         <v>9.2649202163775932</v>
       </c>
     </row>
@@ -2120,37 +2124,37 @@
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <f>POWER(2,A10)*10000000</f>
+        <f t="shared" si="0"/>
         <v>1280000000</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19531.25</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>525.49750017999997</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>506.82523131300002</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>511.57142558300001</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>520.49130418799996</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>495.57018852800002</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>527.18513592900001</v>
       </c>
-      <c r="J10" s="3">
-        <f>AVERAGE(D10:I10)</f>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
         <v>514.52346428683325</v>
       </c>
-      <c r="K10" s="3">
-        <f>_xlfn.STDEV.P(D10:I10)</f>
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
         <v>11.132284065300325</v>
       </c>
     </row>
@@ -2159,35 +2163,35 @@
         <v>8</v>
       </c>
       <c r="B11" s="1">
-        <f>POWER(2,A11)*10000000</f>
+        <f t="shared" si="0"/>
         <v>2560000000</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>39062.5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>997.88241648200005</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1014.7266419809999</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>1005.472644829</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>1062.941862573</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>1051.812781742</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3">
-        <f>AVERAGE(D11:I11)</f>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
         <v>1026.5672695214002</v>
       </c>
-      <c r="K11" s="3">
-        <f>_xlfn.STDEV.P(D11:I11)</f>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
         <v>25.955544117993867</v>
       </c>
     </row>
@@ -2205,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2220,25 +2224,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2247,20 +2251,20 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
       <c r="O2" t="s">
         <v>4</v>
       </c>
@@ -2271,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2439,4 +2443,127 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>158.4082344</v>
+      </c>
+      <c r="C3">
+        <v>228.86222169999999</v>
+      </c>
+      <c r="D3">
+        <v>199.9336131</v>
+      </c>
+      <c r="E3">
+        <v>128.04543860000001</v>
+      </c>
+      <c r="F3">
+        <v>176.9800951</v>
+      </c>
+      <c r="G3">
+        <v>157.98550420000001</v>
+      </c>
+      <c r="H3">
+        <v>94.608490739999993</v>
+      </c>
+      <c r="I3">
+        <v>135.21031139999999</v>
+      </c>
+      <c r="J3">
+        <v>201.8713669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>15.06980602</v>
+      </c>
+      <c r="C4">
+        <v>15.40925161</v>
+      </c>
+      <c r="D4">
+        <v>17.76584875</v>
+      </c>
+      <c r="E4">
+        <v>17.781927639999999</v>
+      </c>
+      <c r="F4">
+        <v>15.12159005</v>
+      </c>
+      <c r="G4">
+        <v>16.098884999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>31.98189648</v>
+      </c>
+      <c r="C5">
+        <v>33.469096290000003</v>
+      </c>
+      <c r="D5">
+        <v>34.162068730000001</v>
+      </c>
+      <c r="E5">
+        <v>35.249737539999998</v>
+      </c>
+      <c r="F5">
+        <v>36.375653909999997</v>
+      </c>
+      <c r="G5">
+        <v>33.53256983</v>
+      </c>
+      <c r="H5">
+        <v>32.552889909999998</v>
+      </c>
+      <c r="I5">
+        <v>33.323034110000002</v>
+      </c>
+      <c r="J5">
+        <v>33.523646769999999</v>
+      </c>
+      <c r="K5">
+        <v>36.897099140000002</v>
+      </c>
+      <c r="L5">
+        <v>35.425754400000002</v>
+      </c>
+      <c r="M5">
+        <v>41.491395019999999</v>
+      </c>
+      <c r="N5">
+        <v>44.18998371</v>
+      </c>
+      <c r="O5">
+        <v>41.468902380000003</v>
+      </c>
+      <c r="P5">
+        <v>43.131554229999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I don't know if anything has changed but I'm committing to be on the safe side.
</commit_message>
<xml_diff>
--- a/benchmark-ec2.xlsx
+++ b/benchmark-ec2.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="14565"/>
+    <workbookView xWindow="480" yWindow="195" windowWidth="27795" windowHeight="14505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="2" r:id="rId1"/>
     <sheet name="scaleout" sheetId="1" r:id="rId2"/>
     <sheet name="scaleup" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Speedup</t>
   </si>
@@ -52,6 +53,24 @@
   </si>
   <si>
     <t>Number of S</t>
+  </si>
+  <si>
+    <t>m1.large</t>
+  </si>
+  <si>
+    <t>m1.xlarge</t>
+  </si>
+  <si>
+    <t>m2.xlarge</t>
+  </si>
+  <si>
+    <t>BoundedMemoryCache</t>
+  </si>
+  <si>
+    <t>WeakReferenceCache</t>
+  </si>
+  <si>
+    <t>SoftReferenceCache</t>
   </si>
 </sst>
 </file>
@@ -832,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97403264"/>
-        <c:axId val="97405184"/>
+        <c:axId val="104502016"/>
+        <c:axId val="104503936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97403264"/>
+        <c:axId val="104502016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,12 +889,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97405184"/>
+        <c:crossAx val="104503936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97405184"/>
+        <c:axId val="104503936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97403264"/>
+        <c:crossAx val="104502016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1011,46 +1030,78 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97618560"/>
-        <c:axId val="97620352"/>
+        <c:axId val="111049728"/>
+        <c:axId val="111059712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97618560"/>
+        <c:axId val="111049728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Instance count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97620352"/>
+        <c:crossAx val="111059712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97620352"/>
+        <c:axId val="111059712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97618560"/>
+        <c:crossAx val="111049728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1078,6 +1129,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iteration time for varying instance count, m1.xlarge. 1.5 GB data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -1189,37 +1255,75 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97641216"/>
-        <c:axId val="97642752"/>
+        <c:axId val="111088768"/>
+        <c:axId val="111090304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97641216"/>
+        <c:axId val="111088768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Instance count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97642752"/>
+        <c:crossAx val="111090304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97642752"/>
+        <c:axId val="111090304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iteration time, seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97641216"/>
+        <c:crossAx val="111088768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1320,11 +1424,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97687424"/>
-        <c:axId val="97688960"/>
+        <c:axId val="111106304"/>
+        <c:axId val="111128576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97687424"/>
+        <c:axId val="111106304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,12 +1438,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97688960"/>
+        <c:crossAx val="111128576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97688960"/>
+        <c:axId val="111128576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97687424"/>
+        <c:crossAx val="111106304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1360,6 +1464,363 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iteration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> times for varying instance type</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>scaleup!$B$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>m1.large</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>m1.xlarge</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>m2.xlarge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>scaleup!$R$3:$R$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>164.65614179333332</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.207884844999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.45168549666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="57870976"/>
+        <c:axId val="57880960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="57870976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Instance type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57880960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="57880960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iteration time, seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57870976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iteration time for varying cache types</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BoundedMemoryCache</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WeakReferenceCache</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SoftReferenceCache</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$1:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>138.40336191566669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125.07967877183334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.406405366666668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="93140096"/>
+        <c:axId val="93142016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93140096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cache type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93142016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93142016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iteration time, seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93140096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1496,6 +1957,76 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1793,7 +2324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
@@ -2210,7 +2741,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,123 +2978,273 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
         <v>158.4082344</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>228.86222169999999</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>199.9336131</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>128.04543860000001</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>176.9800951</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>157.98550420000001</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>94.608490739999993</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>135.21031139999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>201.8713669</v>
       </c>
+      <c r="R3">
+        <f>AVERAGE(C3:Q3)</f>
+        <v>164.65614179333332</v>
+      </c>
+      <c r="S3">
+        <f>_xlfn.STDEV.P(C3:Q3)</f>
+        <v>39.583078834646976</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
         <v>15.06980602</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15.40925161</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>17.76584875</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>17.781927639999999</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>15.12159005</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>16.098884999999999</v>
       </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R5" si="0">AVERAGE(C4:Q4)</f>
+        <v>16.207884844999999</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S5" si="1">_xlfn.STDEV.P(C4:Q4)</f>
+        <v>1.156850469564406</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
         <v>31.98189648</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>33.469096290000003</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>34.162068730000001</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>35.249737539999998</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>36.375653909999997</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>33.53256983</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>32.552889909999998</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>33.323034110000002</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>33.523646769999999</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>36.897099140000002</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>35.425754400000002</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>41.491395019999999</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>44.18998371</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>41.468902380000003</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>43.131554229999999</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>36.45168549666667</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>3.9494754186860668</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" activeCellId="1" sqref="B1:B1048576 I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1">
+        <v>118.14689928599999</v>
+      </c>
+      <c r="D1">
+        <v>133.14645575899999</v>
+      </c>
+      <c r="E1">
+        <v>135.77053987799999</v>
+      </c>
+      <c r="F1">
+        <v>144.415607163</v>
+      </c>
+      <c r="G1">
+        <v>142.39694485199999</v>
+      </c>
+      <c r="H1">
+        <v>156.543724556</v>
+      </c>
+      <c r="I1">
+        <f>AVERAGE(C1:H1)</f>
+        <v>138.40336191566669</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>123.74150791700001</v>
+      </c>
+      <c r="D2">
+        <v>121.936093786</v>
+      </c>
+      <c r="E2">
+        <v>131.04538890399999</v>
+      </c>
+      <c r="F2">
+        <v>127.328765553</v>
+      </c>
+      <c r="G2">
+        <v>128.91505036000001</v>
+      </c>
+      <c r="H2">
+        <v>117.511266111</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I3" si="0">AVERAGE(C2:H2)</f>
+        <v>125.07967877183334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>31.081133263000002</v>
+      </c>
+      <c r="D3">
+        <v>30.453067751999999</v>
+      </c>
+      <c r="E3">
+        <v>34.732923122999999</v>
+      </c>
+      <c r="F3">
+        <v>33.426785445</v>
+      </c>
+      <c r="G3">
+        <v>35.781962720000003</v>
+      </c>
+      <c r="H3">
+        <v>34.962559896999998</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>33.406405366666668</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>